<commit_message>
campo de teste atualizado
</commit_message>
<xml_diff>
--- a/data/SC_001_CampoTeste.xlsx
+++ b/data/SC_001_CampoTeste.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\br-trdkysmgdias\Documents\Repos\KeyFramework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9B7413-0C0C-4A66-85B0-C8F17C97335F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF42C7A2-AD42-4F04-B922-04A0B74870A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,30 +31,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>vExpected Result</t>
   </si>
   <si>
-    <t>vSearch</t>
-  </si>
-  <si>
-    <t>Otter</t>
-  </si>
-  <si>
-    <t>vWrite</t>
-  </si>
-  <si>
     <t>Searched with success</t>
   </si>
   <si>
-    <t>Teste de Escrita</t>
+    <t>vName</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Matheus</t>
+  </si>
+  <si>
+    <t>vLastName</t>
+  </si>
+  <si>
+    <t>Dias</t>
+  </si>
+  <si>
+    <t>vAlertText</t>
+  </si>
+  <si>
+    <t>Era Teste?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,37 +468,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596F6676-CC49-4EAC-B50F-ABE63B457FAA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="27.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved issues with EDGE Driver
</commit_message>
<xml_diff>
--- a/data/SC_001_CampoTeste.xlsx
+++ b/data/SC_001_CampoTeste.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\br-trdkysmgdias\Documents\Repos\KeyFramework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF42C7A2-AD42-4F04-B922-04A0B74870A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEE75B5-855D-423F-9137-95C4A8962F3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001_Access_Campo_Teste" sheetId="1" r:id="rId1"/>
+    <sheet name="TC_002_Teste_Alert_Campo_Teste" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>vExpected Result</t>
   </si>
@@ -40,9 +41,6 @@
   </si>
   <si>
     <t>vName</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Matheus</t>
@@ -470,15 +468,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596F6676-CC49-4EAC-B50F-ABE63B457FAA}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="1" max="4" customWidth="true" width="27.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -486,10 +482,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
@@ -497,13 +493,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -513,4 +509,53 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45D97F7-DB19-4092-9D5F-C516FD03ABFD}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ações com Tabela adicionadas
</commit_message>
<xml_diff>
--- a/data/SC_001_CampoTeste.xlsx
+++ b/data/SC_001_CampoTeste.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\br-trdkysmgdias\Documents\Repos\KeyFramework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEE75B5-855D-423F-9137-95C4A8962F3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F1621E-F4F3-4E4E-883A-3F707E1CD018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001_Access_Campo_Teste" sheetId="1" r:id="rId1"/>
     <sheet name="TC_002_Teste_Alert_Campo_Teste" sheetId="2" r:id="rId2"/>
+    <sheet name="TC_003_Teste_Tabela_Campo_Teste" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>vExpected Result</t>
   </si>
@@ -515,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45D97F7-DB19-4092-9D5F-C516FD03ABFD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,4 +559,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FFB974-AD09-495C-BE7F-6E4562E8ACE5}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added several Table Actions and Nem DataFormat for Key_v13.jar
</commit_message>
<xml_diff>
--- a/data/SC_001_CampoTeste.xlsx
+++ b/data/SC_001_CampoTeste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\br-trdkysmgdias\Documents\Repos\KeyFramework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F1621E-F4F3-4E4E-883A-3F707E1CD018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC484B26-300C-4D2A-9E3C-2F6B3E898CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{E31B522C-28CC-4738-9643-543934F79405}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001_Access_Campo_Teste" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
   <si>
     <t>vExpected Result</t>
   </si>
@@ -516,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45D97F7-DB19-4092-9D5F-C516FD03ABFD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -562,11 +562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FFB974-AD09-495C-BE7F-6E4562E8ACE5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF898FA7-AFD7-4DF3-8681-74862F2FBA2F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>